<commit_message>
Fixed principle violations for inventory patterns
</commit_message>
<xml_diff>
--- a/soa-pattern-analysis.xlsx
+++ b/soa-pattern-analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>Total Patterns</t>
+  </si>
+  <si>
+    <t>Decentralization, Single System, Technological Heterogeneity</t>
   </si>
 </sst>
 </file>
@@ -764,7 +767,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -849,7 +851,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -946,7 +947,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1043,7 +1043,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1089,11 +1088,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1291976848"/>
-        <c:axId val="-1131240912"/>
+        <c:axId val="-500159696"/>
+        <c:axId val="-661460896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1291976848"/>
+        <c:axId val="-500159696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,7 +1132,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1131240912"/>
+        <c:crossAx val="-661460896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1141,7 +1140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1131240912"/>
+        <c:axId val="-661460896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1174,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1291976848"/>
+        <c:crossAx val="-500159696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,7 +1188,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1294,7 +1292,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1379,7 +1376,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1473,7 +1469,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1578,7 +1573,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1683,7 +1677,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1769,7 +1762,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1795,7 +1787,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -1815,11 +1807,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-960840352"/>
-        <c:axId val="-960842528"/>
+        <c:axId val="-497491856"/>
+        <c:axId val="-497489136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-960840352"/>
+        <c:axId val="-497491856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1859,7 +1851,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-960842528"/>
+        <c:crossAx val="-497489136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1867,7 +1859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-960842528"/>
+        <c:axId val="-497489136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +1893,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-960840352"/>
+        <c:crossAx val="-497491856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1915,7 +1907,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3427,7 +3418,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <selection pane="topRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3461,7 +3452,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -3478,10 +3469,10 @@
         <v>154</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3498,7 +3489,7 @@
         <v>155</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5589,7 +5580,7 @@
       </c>
       <c r="H7" s="10">
         <f>G7/SUM(G$7:G$11)</f>
-        <v>0.4375</v>
+        <v>0.42424242424242425</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>2</v>
@@ -5644,7 +5635,7 @@
       </c>
       <c r="H8" s="10">
         <f>G8/SUM(G$7:G$11)</f>
-        <v>0.296875</v>
+        <v>0.2878787878787879</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>34</v>
@@ -5699,7 +5690,7 @@
       </c>
       <c r="H9" s="10">
         <f>G9/SUM(G$7:G$11)</f>
-        <v>0.171875</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>72</v>
@@ -5754,7 +5745,7 @@
       </c>
       <c r="H10" s="10">
         <f>G10/SUM(G$7:G$11)</f>
-        <v>9.375E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>100</v>
@@ -5794,11 +5785,11 @@
       </c>
       <c r="G11">
         <f>COUNTIF('Pattern List'!F$1:F$93, "*"&amp;F11&amp;"*")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="10">
         <f>G11/SUM(G$7:G$11)</f>
-        <v>0</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>115</v>

</xml_diff>